<commit_message>
SPIE2017 Submitted final paper, will still need to create final presentation
</commit_message>
<xml_diff>
--- a/CISC874/Project/PartD/CISC874-0bc15-ProjectPartD/NetworkPerformance.xlsx
+++ b/CISC874/Project/PartD/CISC874-0bc15-ProjectPartD/NetworkPerformance.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Lavenberg-Marquardt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Deletion fraction</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Normalized</t>
+  </si>
+  <si>
+    <t>Testing MAE</t>
+  </si>
+  <si>
+    <t>Validation MAE</t>
+  </si>
+  <si>
+    <t>Training MAE</t>
   </si>
 </sst>
 </file>
@@ -163,6 +172,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Testing Mean Absolute Error</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -215,43 +227,10 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.9099882453343641E-2"/>
-                  <c:y val="0.32599479650196561"/>
+                  <c:x val="-0.26329227251501536"/>
+                  <c:y val="0.17467248908296942"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t>y = 0.1187x + 1.3911</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t>R² = 0.6127</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1200"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -331,37 +310,37 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.30328226</c:v>
+                  <c:v>19.239361600118862</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5640482599999999</c:v>
+                  <c:v>21.740096738030765</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.30363308</c:v>
+                  <c:v>19.24276581904774</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4668761600000002</c:v>
+                  <c:v>21.086478511313221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5174241999999998</c:v>
+                  <c:v>27.535276343664911</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2340986199999997</c:v>
+                  <c:v>25.4981907079157</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3575332600000003</c:v>
+                  <c:v>26.785021859966616</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8482945400000002</c:v>
+                  <c:v>23.9577637103901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.19550482</c:v>
+                  <c:v>25.712709585538516</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.652228</c:v>
+                  <c:v>28.135422506334869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3886489599999998</c:v>
+                  <c:v>27.040128453324151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,6 +352,170 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Training Mean Absolute Error</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.135357712187817"/>
+                  <c:y val="-7.727538424509163E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Lavenberg-Marquardt'!$D$11,'Lavenberg-Marquardt'!$H$11,'Lavenberg-Marquardt'!$L$11,'Lavenberg-Marquardt'!$P$11,'Lavenberg-Marquardt'!$T$11,'Lavenberg-Marquardt'!$X$11,'Lavenberg-Marquardt'!$AB$11,'Lavenberg-Marquardt'!$AF$11,'Lavenberg-Marquardt'!$AJ$11,'Lavenberg-Marquardt'!$AN$11,'Lavenberg-Marquardt'!$AR$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Lavenberg-Marquardt'!$C$73,'Lavenberg-Marquardt'!$G$73,'Lavenberg-Marquardt'!$K$73,'Lavenberg-Marquardt'!$O$73,'Lavenberg-Marquardt'!$S$73,'Lavenberg-Marquardt'!$W$73,'Lavenberg-Marquardt'!$AA$73,'Lavenberg-Marquardt'!$AE$73,'Lavenberg-Marquardt'!$AI$73,'Lavenberg-Marquardt'!$AM$73,'Lavenberg-Marquardt'!$AQ$73)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7.7914107114669449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8833765116237835</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3675597632573488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6187312049853064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.513793516962274</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.88014638498794</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9757212857751103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2442465212309557</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3380232370172909</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7199966505058768</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.244558994369438</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -381,11 +524,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="157867064"/>
-        <c:axId val="157863928"/>
+        <c:axId val="106759104"/>
+        <c:axId val="108180160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157867064"/>
+        <c:axId val="106759104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,12 +650,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157863928"/>
+        <c:crossAx val="108180160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157863928"/>
+        <c:axId val="108180160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,19 +696,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA" sz="1100"/>
-                  <a:t>Average Mean Squared</a:t>
+                  <a:t>Average Mean Absolute </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-                  <a:t> Error (deg</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-CA" sz="1100" baseline="30000"/>
-                  <a:t>2</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-                  <a:t>)</a:t>
+                  <a:t>Error (deg)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA" sz="1100"/>
               </a:p>
@@ -638,7 +773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157867064"/>
+        <c:crossAx val="106759104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -864,37 +999,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.0418522284963234</c:v>
+                  <c:v>7.218593924325007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73538780367365142</c:v>
+                  <c:v>5.5641348554893346</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0416816642410021</c:v>
+                  <c:v>7.2171515798045709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.72250033002512593</c:v>
+                  <c:v>5.2451877619104579</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2523707420669654</c:v>
+                  <c:v>7.2559784299268655</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6043563852196951</c:v>
+                  <c:v>8.4822578901009233</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1510664731392859</c:v>
+                  <c:v>6.4094762449491256</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67427568198032706</c:v>
+                  <c:v>4.4070411839231474</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1326796183704566</c:v>
+                  <c:v>6.7838131009497609</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3594251876732011</c:v>
+                  <c:v>7.96596652362937</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0467784475970925</c:v>
+                  <c:v>6.0735419308971927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,11 +1044,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="207713296"/>
-        <c:axId val="207712904"/>
+        <c:axId val="108178984"/>
+        <c:axId val="108178200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="207713296"/>
+        <c:axId val="108178984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,12 +1170,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207712904"/>
+        <c:crossAx val="108178200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="207712904"/>
+        <c:axId val="108178200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,7 +1293,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207713296"/>
+        <c:crossAx val="108178984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2324,15 +2459,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2353,16 +2488,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2649,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AS74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q17" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4250,13 +4385,13 @@
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
@@ -4264,146 +4399,146 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <f>C16*180</f>
-        <v>0.15410573999999999</v>
+        <f t="shared" ref="C47:D47" si="6">SQRT(C16)*240</f>
+        <v>7.0223811346294776</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" ref="D47:E47" si="6">D16*180</f>
-        <v>1.1627334</v>
+        <f t="shared" si="6"/>
+        <v>19.289237621015509</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="6"/>
-        <v>1.1145006</v>
+        <f>SQRT(E16)*240</f>
+        <v>18.884919698002424</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1">
-        <f t="shared" ref="G47:L47" si="7">G16*180</f>
-        <v>0.63022319999999998</v>
+        <f t="shared" ref="G47:AS47" si="7">SQRT(G16)*240</f>
+        <v>14.201106435767603</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="7"/>
-        <v>1.839294</v>
+        <v>24.260545748189589</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="7"/>
-        <v>1.1373390000000001</v>
+        <v>19.077433789689849</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1">
         <f t="shared" si="7"/>
-        <v>0.15410573999999999</v>
+        <v>7.0223811346294776</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="7"/>
-        <v>1.1627334</v>
+        <v>19.289237621015509</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47" si="8">M16*180</f>
-        <v>1.1144826000000001</v>
+        <f t="shared" si="7"/>
+        <v>18.884767194752495</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1">
-        <f t="shared" ref="O47:S47" si="9">O16*180</f>
-        <v>1.4536907999999999</v>
+        <f t="shared" si="7"/>
+        <v>21.568056379748271</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" si="9"/>
-        <v>2.5925579999999999</v>
+        <f t="shared" si="7"/>
+        <v>28.803099833177679</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" si="9"/>
-        <v>2.0408219999999999</v>
+        <f t="shared" si="7"/>
+        <v>25.555098121509925</v>
       </c>
       <c r="R47" s="1"/>
       <c r="S47" s="1">
-        <f t="shared" si="9"/>
-        <v>1.808478</v>
+        <f t="shared" si="7"/>
+        <v>24.056453603970805</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" ref="T47" si="10">T16*180</f>
-        <v>1.4540382000000001</v>
+        <f t="shared" si="7"/>
+        <v>21.570633370395036</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" ref="U47:W47" si="11">U16*180</f>
-        <v>2.928474</v>
+        <f t="shared" si="7"/>
+        <v>30.612279888959595</v>
       </c>
       <c r="V47" s="1"/>
       <c r="W47" s="1">
-        <f t="shared" si="11"/>
-        <v>1.2390371999999998</v>
+        <f t="shared" si="7"/>
+        <v>19.912104459348338</v>
       </c>
       <c r="X47" s="1">
-        <f t="shared" ref="X47:Y47" si="12">X16*180</f>
-        <v>1.1178306</v>
+        <f t="shared" si="7"/>
+        <v>18.913111642455874</v>
       </c>
       <c r="Y47" s="1">
-        <f t="shared" si="12"/>
-        <v>6.2343900000000003</v>
+        <f t="shared" si="7"/>
+        <v>44.665476601061805</v>
       </c>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1">
-        <f t="shared" ref="AA47:AS47" si="13">AA16*180</f>
-        <v>2.7871199999999999E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.9864333242180376</v>
       </c>
       <c r="AB47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.4370227999999998</v>
+        <f t="shared" si="7"/>
+        <v>21.444050363678969</v>
       </c>
       <c r="AC47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.3665402</v>
+        <f t="shared" si="7"/>
+        <v>20.911548579672431</v>
       </c>
       <c r="AD47" s="1"/>
       <c r="AE47" s="1">
-        <f t="shared" si="13"/>
-        <v>0.14031360000000001</v>
+        <f t="shared" si="7"/>
+        <v>6.7007724927802164</v>
       </c>
       <c r="AF47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.564587</v>
+        <f t="shared" si="7"/>
+        <v>22.375608148159905</v>
       </c>
       <c r="AG47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.1640654000000001</v>
+        <f t="shared" si="7"/>
+        <v>19.300283106731879</v>
       </c>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1">
-        <f t="shared" si="13"/>
-        <v>4.526118E-3</v>
+        <f t="shared" si="7"/>
+        <v>1.2034773616483194</v>
       </c>
       <c r="AJ47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.818522</v>
+        <f t="shared" si="7"/>
+        <v>24.123163971585484</v>
       </c>
       <c r="AK47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.3012632</v>
+        <f t="shared" si="7"/>
+        <v>20.405985004404958</v>
       </c>
       <c r="AL47" s="1"/>
       <c r="AM47" s="1">
-        <f t="shared" si="13"/>
-        <v>0.16160075999999998</v>
+        <f t="shared" si="7"/>
+        <v>7.1911225271163328</v>
       </c>
       <c r="AN47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.2262751999999999</v>
+        <f t="shared" si="7"/>
+        <v>19.809292364948323</v>
       </c>
       <c r="AO47" s="1">
-        <f t="shared" si="13"/>
-        <v>0.77991480000000002</v>
+        <f t="shared" si="7"/>
+        <v>15.797871249000607</v>
       </c>
       <c r="AP47" s="1"/>
       <c r="AQ47" s="1">
-        <f t="shared" si="13"/>
-        <v>0.1081458</v>
+        <f t="shared" si="7"/>
+        <v>5.8827422177076567</v>
       </c>
       <c r="AR47" s="1">
-        <f t="shared" si="13"/>
-        <v>2.8608480000000003</v>
+        <f t="shared" si="7"/>
+        <v>30.256757261808477</v>
       </c>
       <c r="AS47" s="1">
-        <f t="shared" si="13"/>
-        <v>1.5718122000000001</v>
+        <f t="shared" si="7"/>
+        <v>22.427213469354591</v>
       </c>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
@@ -4411,146 +4546,146 @@
         <v>2</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ref="C48:E56" si="14">C17*180</f>
-        <v>0.12688991999999999</v>
+        <f t="shared" ref="C48:E56" si="8">SQRT(C17)*240</f>
+        <v>6.3721875678608209</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="14"/>
-        <v>0.81927179999999999</v>
+        <f t="shared" si="8"/>
+        <v>16.191571140565696</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="14"/>
-        <v>0.94563180000000002</v>
+        <f t="shared" si="8"/>
+        <v>17.395464236403694</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1">
-        <f t="shared" ref="G48:L48" si="15">G17*180</f>
-        <v>0.64060019999999995</v>
+        <f t="shared" ref="G48:AS48" si="9">SQRT(G17)*240</f>
+        <v>14.317543923452794</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="15"/>
-        <v>0.79285859999999997</v>
+        <f t="shared" si="9"/>
+        <v>15.928425910930432</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="15"/>
-        <v>2.0070360000000003</v>
+        <f t="shared" si="9"/>
+        <v>25.342681783899668</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1">
-        <f t="shared" si="15"/>
-        <v>0.12688991999999999</v>
+        <f t="shared" si="9"/>
+        <v>6.3721875678608209</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" si="15"/>
-        <v>0.81927179999999999</v>
+        <f t="shared" si="9"/>
+        <v>16.191571140565696</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" ref="M48" si="16">M17*180</f>
-        <v>0.94563180000000002</v>
+        <f t="shared" si="9"/>
+        <v>17.395464236403694</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1">
-        <f t="shared" ref="O48:S48" si="17">O17*180</f>
-        <v>0.20832299999999998</v>
+        <f t="shared" si="9"/>
+        <v>8.1647633156142376</v>
       </c>
       <c r="P48" s="1">
-        <f t="shared" si="17"/>
-        <v>2.3605200000000002</v>
+        <f t="shared" si="9"/>
+        <v>27.483929850005076</v>
       </c>
       <c r="Q48" s="1">
-        <f t="shared" si="17"/>
-        <v>2.2388759999999999</v>
+        <f t="shared" si="9"/>
+        <v>26.766402821447638</v>
       </c>
       <c r="R48" s="1"/>
       <c r="S48" s="1">
-        <f t="shared" si="17"/>
-        <v>2.0919419999999997E-6</v>
+        <f t="shared" si="9"/>
+        <v>2.587317993598777E-2</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" ref="T48" si="18">T17*180</f>
-        <v>3.9816000000000003</v>
+        <f t="shared" si="9"/>
+        <v>35.694705489750156</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" ref="U48:W48" si="19">U17*180</f>
-        <v>4.0987079999999994</v>
+        <f t="shared" si="9"/>
+        <v>36.215833001603045</v>
       </c>
       <c r="V48" s="1"/>
       <c r="W48" s="1">
-        <f t="shared" si="19"/>
-        <v>1.0438829999999999</v>
+        <f t="shared" si="9"/>
+        <v>18.276831235200483</v>
       </c>
       <c r="X48" s="1">
-        <f t="shared" ref="X48:Y48" si="20">X17*180</f>
-        <v>0.72154080000000009</v>
+        <f t="shared" si="9"/>
+        <v>15.19516554697579</v>
       </c>
       <c r="Y48" s="1">
-        <f t="shared" si="20"/>
-        <v>2.0100959999999999</v>
+        <f t="shared" si="9"/>
+        <v>25.361993612490323</v>
       </c>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1">
-        <f t="shared" ref="AA48:AS48" si="21">AA17*180</f>
-        <v>2.233566E-13</v>
+        <f t="shared" si="9"/>
+        <v>8.4542363345248404E-6</v>
       </c>
       <c r="AB48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.5360552000000001</v>
+        <f t="shared" si="9"/>
+        <v>22.170648704988313</v>
       </c>
       <c r="AC48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.8489779999999998</v>
+        <f t="shared" si="9"/>
+        <v>24.324328562161792</v>
       </c>
       <c r="AD48" s="1"/>
       <c r="AE48" s="1">
-        <f t="shared" si="21"/>
-        <v>0.28091520000000003</v>
+        <f t="shared" si="9"/>
+        <v>9.4811847360970667</v>
       </c>
       <c r="AF48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.1501838</v>
+        <f t="shared" si="9"/>
+        <v>19.184859029974653</v>
       </c>
       <c r="AG48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.8516240000000002</v>
+        <f t="shared" si="9"/>
+        <v>24.34172713675018</v>
       </c>
       <c r="AH48" s="1"/>
       <c r="AI48" s="1">
-        <f t="shared" si="21"/>
-        <v>8.2683000000000008E-4</v>
+        <f t="shared" si="9"/>
+        <v>0.51437884870978123</v>
       </c>
       <c r="AJ48" s="1">
-        <f t="shared" si="21"/>
-        <v>0.75729239999999998</v>
+        <f t="shared" si="9"/>
+        <v>15.567066775728817</v>
       </c>
       <c r="AK48" s="1">
-        <f t="shared" si="21"/>
-        <v>0.926118</v>
+        <f t="shared" si="9"/>
+        <v>17.215044583154583</v>
       </c>
       <c r="AL48" s="1"/>
       <c r="AM48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.325745</v>
+        <f t="shared" si="9"/>
+        <v>20.597048332224691</v>
       </c>
       <c r="AN48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.4034203999999999</v>
+        <f t="shared" si="9"/>
+        <v>21.191850509099009</v>
       </c>
       <c r="AO48" s="1">
-        <f t="shared" si="21"/>
-        <v>3.1861439999999996</v>
+        <f t="shared" si="9"/>
+        <v>31.930644841593789</v>
       </c>
       <c r="AP48" s="1"/>
       <c r="AQ48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.2233088E-2</v>
+        <f t="shared" si="9"/>
+        <v>1.9785318193044052</v>
       </c>
       <c r="AR48" s="1">
-        <f t="shared" si="21"/>
-        <v>1.698021</v>
+        <f t="shared" si="9"/>
+        <v>23.310227798114717</v>
       </c>
       <c r="AS48" s="1">
-        <f t="shared" si="21"/>
-        <v>2.8222199999999997</v>
+        <f t="shared" si="9"/>
+        <v>30.051795287469933</v>
       </c>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.25">
@@ -4558,146 +4693,146 @@
         <v>3</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="14"/>
-        <v>0.17258184000000001</v>
+        <f t="shared" si="8"/>
+        <v>7.4314324864052956</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="14"/>
-        <v>1.256769</v>
+        <f t="shared" si="8"/>
+        <v>20.054078886849926</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="14"/>
-        <v>0.61898039999999999</v>
+        <f t="shared" si="8"/>
+        <v>14.073866846037729</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1">
-        <f t="shared" ref="G49:L49" si="22">G18*180</f>
-        <v>0.2579436</v>
+        <f t="shared" ref="G49:AS49" si="10">SQRT(G18)*240</f>
+        <v>9.0852601503754418</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="22"/>
-        <v>2.37087</v>
+        <f t="shared" si="10"/>
+        <v>27.544117339279545</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="22"/>
-        <v>1.6277309999999998</v>
+        <f t="shared" si="10"/>
+        <v>22.822662421374066</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1">
-        <f t="shared" si="22"/>
-        <v>0.17258184000000001</v>
+        <f t="shared" si="10"/>
+        <v>7.4314324864052956</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="22"/>
-        <v>1.256769</v>
+        <f t="shared" si="10"/>
+        <v>20.054078886849926</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" ref="M49" si="23">M18*180</f>
-        <v>0.61898039999999999</v>
+        <f t="shared" si="10"/>
+        <v>14.073866846037729</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1">
-        <f t="shared" ref="O49:S49" si="24">O18*180</f>
-        <v>8.2439279999999995E-10</v>
+        <f t="shared" si="10"/>
+        <v>5.136201865191827E-4</v>
       </c>
       <c r="P49" s="1">
-        <f t="shared" si="24"/>
-        <v>0.63984779999999997</v>
+        <f t="shared" si="10"/>
+        <v>14.309133307087469</v>
       </c>
       <c r="Q49" s="1">
-        <f t="shared" si="24"/>
-        <v>0.79357500000000003</v>
+        <f t="shared" si="10"/>
+        <v>15.935620477408467</v>
       </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1">
-        <f t="shared" si="24"/>
-        <v>0.57107340000000006</v>
+        <f t="shared" si="10"/>
+        <v>13.518264977429611</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" ref="T49" si="25">T18*180</f>
-        <v>1.573083</v>
+        <f t="shared" si="10"/>
+        <v>22.436277766153633</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" ref="U49:W49" si="26">U18*180</f>
-        <v>3.857526</v>
+        <f t="shared" si="10"/>
+        <v>35.134147492147861</v>
       </c>
       <c r="V49" s="1"/>
       <c r="W49" s="1">
-        <f t="shared" si="26"/>
-        <v>2.1832200000000002E-9</v>
+        <f t="shared" si="10"/>
+        <v>8.3584113323047226E-4</v>
       </c>
       <c r="X49" s="1">
-        <f t="shared" ref="X49:Y49" si="27">X18*180</f>
-        <v>1.9639979999999999</v>
+        <f t="shared" si="10"/>
+        <v>25.069490621071662</v>
       </c>
       <c r="Y49" s="1">
-        <f t="shared" si="27"/>
-        <v>2.260062</v>
+        <f t="shared" si="10"/>
+        <v>26.892746977577428</v>
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1">
-        <f t="shared" ref="AA49:AS49" si="28">AA18*180</f>
-        <v>1.2021390000000001</v>
+        <f t="shared" si="10"/>
+        <v>19.613375028281084</v>
       </c>
       <c r="AB49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.8451439999999999</v>
+        <f t="shared" si="10"/>
+        <v>24.299096279491547</v>
       </c>
       <c r="AC49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.532762</v>
+        <f t="shared" si="10"/>
+        <v>28.468997874881371</v>
       </c>
       <c r="AD49" s="1"/>
       <c r="AE49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.1209500000000001</v>
+        <f t="shared" si="10"/>
+        <v>18.939482569489591</v>
       </c>
       <c r="AF49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.7886294</v>
+        <f t="shared" si="10"/>
+        <v>23.924075906918539</v>
       </c>
       <c r="AG49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.8182340000000001</v>
+        <f t="shared" si="10"/>
+        <v>24.121253698761183</v>
       </c>
       <c r="AH49" s="1"/>
       <c r="AI49" s="1">
-        <f t="shared" si="28"/>
-        <v>0.95198939999999987</v>
+        <f t="shared" si="10"/>
+        <v>17.453842213105972</v>
       </c>
       <c r="AJ49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.106198</v>
+        <f t="shared" si="10"/>
+        <v>25.961189495090551</v>
       </c>
       <c r="AK49" s="1">
-        <f t="shared" si="28"/>
-        <v>3.3058440000000004</v>
+        <f t="shared" si="10"/>
+        <v>32.524914757766858</v>
       </c>
       <c r="AL49" s="1"/>
       <c r="AM49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.1813454000000001</v>
+        <f t="shared" si="10"/>
+        <v>19.443007174817378</v>
       </c>
       <c r="AN49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.00502</v>
+        <f t="shared" si="10"/>
+        <v>25.329950651353428</v>
       </c>
       <c r="AO49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.0206080000000002</v>
+        <f t="shared" si="10"/>
+        <v>25.428223689436116</v>
       </c>
       <c r="AP49" s="1"/>
       <c r="AQ49" s="1">
-        <f t="shared" si="28"/>
-        <v>1.9545660000000002E-5</v>
+        <f t="shared" si="10"/>
+        <v>7.9086099916483438E-2</v>
       </c>
       <c r="AR49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.7931319999999999</v>
+        <f t="shared" si="10"/>
+        <v>29.896525550638824</v>
       </c>
       <c r="AS49" s="1">
-        <f t="shared" si="28"/>
-        <v>2.0059559999999999</v>
+        <f t="shared" si="10"/>
+        <v>25.335862329906988</v>
       </c>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.25">
@@ -4705,146 +4840,146 @@
         <v>4</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="14"/>
-        <v>7.7318460000000006E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.9741237620308558</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="14"/>
-        <v>1.0074114000000001</v>
+        <f t="shared" si="8"/>
+        <v>17.954711025243487</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="14"/>
-        <v>0.480375</v>
+        <f t="shared" si="8"/>
+        <v>12.398386991863095</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1">
-        <f t="shared" ref="G50:L50" si="29">G19*180</f>
-        <v>6.2167500000000001E-3</v>
+        <f t="shared" ref="G50:AS50" si="11">SQRT(G19)*240</f>
+        <v>1.4104467377395009</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="29"/>
-        <v>0.31161060000000002</v>
+        <f t="shared" si="11"/>
+        <v>9.9857594603515274</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="29"/>
-        <v>1.0717920000000001</v>
+        <f t="shared" si="11"/>
+        <v>18.519542110970239</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1">
-        <f t="shared" si="29"/>
-        <v>7.7318460000000006E-2</v>
+        <f t="shared" si="11"/>
+        <v>4.9741237620308558</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" si="29"/>
-        <v>1.0074114000000001</v>
+        <f t="shared" si="11"/>
+        <v>17.954711025243487</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" ref="M50" si="30">M19*180</f>
-        <v>0.48034259999999995</v>
+        <f t="shared" si="11"/>
+        <v>12.397968865907028</v>
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1">
-        <f t="shared" ref="O50:S50" si="31">O19*180</f>
-        <v>2.2136039999999999E-2</v>
+        <f t="shared" si="11"/>
+        <v>2.6614907101096557</v>
       </c>
       <c r="P50" s="1">
-        <f t="shared" si="31"/>
-        <v>2.0511900000000001</v>
+        <f t="shared" si="11"/>
+        <v>25.619929742292424</v>
       </c>
       <c r="Q50" s="1">
-        <f t="shared" si="31"/>
-        <v>0.9731592</v>
+        <f t="shared" si="11"/>
+        <v>17.646839490401671</v>
       </c>
       <c r="R50" s="1"/>
       <c r="S50" s="1">
-        <f t="shared" si="31"/>
-        <v>1.0970424000000001</v>
+        <f t="shared" si="11"/>
+        <v>18.736423564810867</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" ref="T50" si="32">T19*180</f>
-        <v>0.83451419999999998</v>
+        <f t="shared" si="11"/>
+        <v>16.341497605788767</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" ref="U50:W50" si="33">U19*180</f>
-        <v>1.5203159999999998</v>
+        <f t="shared" si="11"/>
+        <v>22.056770389157158</v>
       </c>
       <c r="V50" s="1"/>
       <c r="W50" s="1">
-        <f t="shared" si="33"/>
-        <v>0.17020259999999998</v>
+        <f t="shared" si="11"/>
+        <v>7.3800292682346456</v>
       </c>
       <c r="X50" s="1">
-        <f t="shared" ref="X50:Y50" si="34">X19*180</f>
-        <v>1.258542</v>
+        <f t="shared" si="11"/>
+        <v>20.068219651977103</v>
       </c>
       <c r="Y50" s="1">
-        <f t="shared" si="34"/>
-        <v>1.0401875999999999</v>
+        <f t="shared" si="11"/>
+        <v>18.244452088237672</v>
       </c>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1">
-        <f t="shared" ref="AA50:AS50" si="35">AA19*180</f>
-        <v>1.2539303999999999E-2</v>
+        <f t="shared" si="11"/>
+        <v>2.0031418521912023</v>
       </c>
       <c r="AB50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.0587978</v>
+        <f t="shared" si="11"/>
+        <v>18.406936083987468</v>
       </c>
       <c r="AC50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.391076</v>
+        <f t="shared" si="11"/>
+        <v>21.09844354448925</v>
       </c>
       <c r="AD50" s="1"/>
       <c r="AE50" s="1">
-        <f t="shared" si="35"/>
-        <v>3.86244E-20</v>
+        <f t="shared" si="11"/>
+        <v>3.5156518598973928E-9</v>
       </c>
       <c r="AF50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.9424700000000001</v>
+        <f t="shared" si="11"/>
+        <v>24.931714742472085</v>
       </c>
       <c r="AG50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.020645</v>
+        <f t="shared" si="11"/>
+        <v>18.072254978280935</v>
       </c>
       <c r="AH50" s="1"/>
       <c r="AI50" s="1">
-        <f t="shared" si="35"/>
-        <v>6.9922980000000001E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.4958393496629241</v>
       </c>
       <c r="AJ50" s="1">
-        <f t="shared" si="35"/>
-        <v>2.113092</v>
+        <f t="shared" si="11"/>
+        <v>26.00364282172788</v>
       </c>
       <c r="AK50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.0662192000000001</v>
+        <f t="shared" si="11"/>
+        <v>18.471333032566978</v>
       </c>
       <c r="AL50" s="1"/>
       <c r="AM50" s="1">
-        <f t="shared" si="35"/>
-        <v>6.884154E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.4842268290258063</v>
       </c>
       <c r="AN50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.4004342000000001</v>
+        <f t="shared" si="11"/>
+        <v>21.169292477548701</v>
       </c>
       <c r="AO50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.6849871999999999</v>
+        <f t="shared" si="11"/>
+        <v>23.220592240509283</v>
       </c>
       <c r="AP50" s="1"/>
       <c r="AQ50" s="1">
-        <f t="shared" si="35"/>
-        <v>0.74849220000000005</v>
+        <f t="shared" si="11"/>
+        <v>15.47635305877971</v>
       </c>
       <c r="AR50" s="1">
-        <f t="shared" si="35"/>
-        <v>2.4322319999999999</v>
+        <f t="shared" si="11"/>
+        <v>27.898283818184947</v>
       </c>
       <c r="AS50" s="1">
-        <f t="shared" si="35"/>
-        <v>1.9322099999999998</v>
+        <f t="shared" si="11"/>
+        <v>24.865783719802597</v>
       </c>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.25">
@@ -4852,146 +4987,146 @@
         <v>5</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="14"/>
-        <v>3.0353580000000002E-3</v>
+        <f t="shared" si="8"/>
+        <v>0.98555292095351221</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="14"/>
-        <v>1.2488147999999999</v>
+        <f t="shared" si="8"/>
+        <v>19.990516151415402</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="14"/>
-        <v>2.2918500000000002</v>
+        <f t="shared" si="8"/>
+        <v>27.081211198910584</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1">
-        <f t="shared" ref="G51:L51" si="36">G20*180</f>
-        <v>0.19975859999999998</v>
+        <f t="shared" ref="G51:AS51" si="12">SQRT(G20)*240</f>
+        <v>7.9951705422711274</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="36"/>
-        <v>0.84091319999999992</v>
+        <f t="shared" si="12"/>
+        <v>16.404030724184835</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="36"/>
-        <v>1.8437400000000002</v>
+        <f t="shared" si="12"/>
+        <v>24.289849731935355</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1">
-        <f t="shared" si="36"/>
-        <v>3.0353580000000002E-3</v>
+        <f t="shared" si="12"/>
+        <v>0.98555292095351221</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="36"/>
-        <v>1.2488147999999999</v>
+        <f t="shared" si="12"/>
+        <v>19.990516151415402</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" ref="M51" si="37">M20*180</f>
-        <v>2.2918500000000002</v>
+        <f t="shared" si="12"/>
+        <v>27.081211198910584</v>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1">
-        <f t="shared" ref="O51:S51" si="38">O20*180</f>
-        <v>4.8830039999999998E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.2500245117596693</v>
       </c>
       <c r="P51" s="1">
-        <f t="shared" si="38"/>
-        <v>0.36663840000000003</v>
+        <f t="shared" si="12"/>
+        <v>10.831633671796698</v>
       </c>
       <c r="Q51" s="1">
-        <f t="shared" si="38"/>
-        <v>0.85451220000000006</v>
+        <f t="shared" si="12"/>
+        <v>16.536139331778745</v>
       </c>
       <c r="R51" s="1"/>
       <c r="S51" s="1">
-        <f t="shared" si="38"/>
-        <v>1.0414782</v>
+        <f t="shared" si="12"/>
+        <v>18.255766869677103</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" ref="T51" si="39">T20*180</f>
-        <v>3.8180519999999998</v>
+        <f t="shared" si="12"/>
+        <v>34.953921668390805</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" ref="U51:W51" si="40">U20*180</f>
-        <v>1.260459</v>
+        <f t="shared" si="12"/>
+        <v>20.083497703338431</v>
       </c>
       <c r="V51" s="1"/>
       <c r="W51" s="1">
-        <f t="shared" si="40"/>
-        <v>0.24118560000000003</v>
+        <f t="shared" si="12"/>
+        <v>8.7851802485777153</v>
       </c>
       <c r="X51" s="1">
-        <f t="shared" ref="X51:Y51" si="41">X20*180</f>
-        <v>0.89552700000000007</v>
+        <f t="shared" si="12"/>
+        <v>16.928338370909294</v>
       </c>
       <c r="Y51" s="1">
-        <f t="shared" si="41"/>
-        <v>1.3547988</v>
+        <f t="shared" si="12"/>
+        <v>20.821518100273092</v>
       </c>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1">
-        <f t="shared" ref="AA51:AS51" si="42">AA20*180</f>
-        <v>3.5557200000000002E-4</v>
+        <f t="shared" si="12"/>
+        <v>0.33731741727933351</v>
       </c>
       <c r="AB51" s="1">
-        <f t="shared" si="42"/>
-        <v>1.2774923999999999</v>
+        <f t="shared" si="12"/>
+        <v>20.218742987634023</v>
       </c>
       <c r="AC51" s="1">
-        <f t="shared" si="42"/>
-        <v>2.3423400000000001</v>
+        <f t="shared" si="12"/>
+        <v>27.377888888663421</v>
       </c>
       <c r="AD51" s="1"/>
       <c r="AE51" s="1">
-        <f t="shared" si="42"/>
-        <v>0.12055896000000001</v>
+        <f t="shared" si="12"/>
+        <v>6.2111888717056418</v>
       </c>
       <c r="AF51" s="1">
-        <f t="shared" si="42"/>
-        <v>1.7582705999999999</v>
+        <f t="shared" si="12"/>
+        <v>23.720172680653064</v>
       </c>
       <c r="AG51" s="1">
-        <f t="shared" si="42"/>
-        <v>1.7591292000000001</v>
+        <f t="shared" si="12"/>
+        <v>23.725963499929779</v>
       </c>
       <c r="AH51" s="1"/>
       <c r="AI51" s="1">
-        <f t="shared" si="42"/>
-        <v>0.27229140000000002</v>
+        <f t="shared" si="12"/>
+        <v>9.334519162763554</v>
       </c>
       <c r="AJ51" s="1">
-        <f t="shared" si="42"/>
-        <v>1.6603056</v>
+        <f t="shared" si="12"/>
+        <v>23.049897873960312</v>
       </c>
       <c r="AK51" s="1">
-        <f t="shared" si="42"/>
-        <v>3.020292</v>
+        <f t="shared" si="12"/>
+        <v>31.088477608271525</v>
       </c>
       <c r="AL51" s="1"/>
       <c r="AM51" s="1">
-        <f t="shared" si="42"/>
-        <v>9.4412879999999991E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.7381634445586525</v>
       </c>
       <c r="AN51" s="1">
-        <f t="shared" si="42"/>
-        <v>2.5619040000000002</v>
+        <f t="shared" si="12"/>
+        <v>28.632311817245913</v>
       </c>
       <c r="AO51" s="1">
-        <f t="shared" si="42"/>
-        <v>3.246966</v>
+        <f t="shared" si="12"/>
+        <v>32.23397462305882</v>
       </c>
       <c r="AP51" s="1"/>
       <c r="AQ51" s="1">
-        <f t="shared" si="42"/>
-        <v>0.22006980000000001</v>
+        <f t="shared" si="12"/>
+        <v>8.3918017135773653</v>
       </c>
       <c r="AR51" s="1">
-        <f t="shared" si="42"/>
-        <v>2.3540399999999999</v>
+        <f t="shared" si="12"/>
+        <v>27.446180062077858</v>
       </c>
       <c r="AS51" s="1">
-        <f t="shared" si="42"/>
-        <v>1.7562114</v>
+        <f t="shared" si="12"/>
+        <v>23.706278661991636</v>
       </c>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.25">
@@ -4999,146 +5134,146 @@
         <v>6</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="14"/>
-        <v>7.6362659999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.9432834432186867</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="14"/>
-        <v>1.664838</v>
+        <f t="shared" si="8"/>
+        <v>23.081337916160752</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="14"/>
-        <v>1.3195547999999999</v>
+        <f t="shared" si="8"/>
+        <v>20.548905956279036</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1">
-        <f t="shared" ref="G52:L52" si="43">G21*180</f>
-        <v>0.19714139999999999</v>
+        <f t="shared" ref="G52:AS52" si="13">SQRT(G21)*240</f>
+        <v>7.9426222370197106</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="43"/>
-        <v>0.27898200000000001</v>
+        <f t="shared" si="13"/>
+        <v>9.4485046435930808</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="43"/>
-        <v>0.69978240000000003</v>
+        <f t="shared" si="13"/>
+        <v>14.964303124435833</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1">
-        <f t="shared" si="43"/>
-        <v>7.6362659999999999E-2</v>
+        <f t="shared" si="13"/>
+        <v>4.9432834432186867</v>
       </c>
       <c r="L52" s="1">
-        <f t="shared" si="43"/>
-        <v>1.664838</v>
+        <f t="shared" si="13"/>
+        <v>23.081337916160752</v>
       </c>
       <c r="M52" s="1">
-        <f t="shared" ref="M52" si="44">M21*180</f>
-        <v>1.3195547999999999</v>
+        <f t="shared" si="13"/>
+        <v>20.548905956279036</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1">
-        <f t="shared" ref="O52:S52" si="45">O21*180</f>
-        <v>3.8764080000000002E-5</v>
+        <f t="shared" si="13"/>
+        <v>0.11137551616042012</v>
       </c>
       <c r="P52" s="1">
-        <f t="shared" si="45"/>
-        <v>0.4060242</v>
+        <f t="shared" si="13"/>
+        <v>11.398585175362774</v>
       </c>
       <c r="Q52" s="1">
-        <f t="shared" si="45"/>
-        <v>1.5509196000000001</v>
+        <f t="shared" si="13"/>
+        <v>22.277663073132246</v>
       </c>
       <c r="R52" s="1"/>
       <c r="S52" s="1">
-        <f t="shared" si="45"/>
-        <v>2.9024819999999997E-6</v>
+        <f t="shared" si="13"/>
+        <v>3.047612573802648E-2</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" ref="T52" si="46">T21*180</f>
-        <v>1.903356</v>
+        <f t="shared" si="13"/>
+        <v>24.679423007841976</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" ref="U52:W52" si="47">U21*180</f>
-        <v>1.6143785999999998</v>
+        <f t="shared" si="13"/>
+        <v>22.728861652093357</v>
       </c>
       <c r="V52" s="1"/>
       <c r="W52" s="1">
-        <f t="shared" si="47"/>
-        <v>7.2941219999999995E-8</v>
+        <f t="shared" si="13"/>
+        <v>4.8312721306090801E-3</v>
       </c>
       <c r="X52" s="1">
-        <f t="shared" ref="X52:Y52" si="48">X21*180</f>
-        <v>2.3459219999999998</v>
+        <f t="shared" si="13"/>
+        <v>27.398814572897127</v>
       </c>
       <c r="Y52" s="1">
-        <f t="shared" si="48"/>
-        <v>2.849904</v>
+        <f t="shared" si="13"/>
+        <v>30.198829116374696</v>
       </c>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1">
-        <f t="shared" ref="AA52:AS52" si="49">AA21*180</f>
-        <v>8.750376E-2</v>
+        <f t="shared" si="13"/>
+        <v>5.2916163126213149</v>
       </c>
       <c r="AB52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.7694468000000001</v>
+        <f t="shared" si="13"/>
+        <v>23.795440235473684</v>
       </c>
       <c r="AC52" s="1">
-        <f t="shared" si="49"/>
-        <v>2.9199600000000001</v>
+        <f t="shared" si="13"/>
+        <v>30.56774770898242</v>
       </c>
       <c r="AD52" s="1"/>
       <c r="AE52" s="1">
-        <f t="shared" si="49"/>
-        <v>3.8398680000000004E-2</v>
+        <f t="shared" si="13"/>
+        <v>3.5053641180339601</v>
       </c>
       <c r="AF52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.5539328000000001</v>
+        <f t="shared" si="13"/>
+        <v>22.299293621099302</v>
       </c>
       <c r="AG52" s="1">
-        <f t="shared" si="49"/>
-        <v>2.0495700000000001</v>
+        <f t="shared" si="13"/>
+        <v>25.60981062015102</v>
       </c>
       <c r="AH52" s="1"/>
       <c r="AI52" s="1">
-        <f t="shared" si="49"/>
-        <v>2.7261180000000003E-2</v>
+        <f t="shared" si="13"/>
+        <v>2.9535703140436662</v>
       </c>
       <c r="AJ52" s="1">
-        <f t="shared" si="49"/>
-        <v>0.87576659999999995</v>
+        <f t="shared" si="13"/>
+        <v>16.740529023898855</v>
       </c>
       <c r="AK52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.9360439999999999</v>
+        <f t="shared" si="13"/>
+        <v>24.890441538871904</v>
       </c>
       <c r="AL52" s="1"/>
       <c r="AM52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.0769561999999999E-3</v>
+        <f t="shared" si="13"/>
+        <v>0.58704853632387155</v>
       </c>
       <c r="AN52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.5645006000000001</v>
+        <f t="shared" si="13"/>
+        <v>22.374990324020253</v>
       </c>
       <c r="AO52" s="1">
-        <f t="shared" si="49"/>
-        <v>2.19339</v>
+        <f t="shared" si="13"/>
+        <v>26.493108537882073</v>
       </c>
       <c r="AP52" s="1"/>
       <c r="AQ52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.8072000000000001E-2</v>
+        <f t="shared" si="13"/>
+        <v>2.4047952095760667</v>
       </c>
       <c r="AR52" s="1">
-        <f t="shared" si="49"/>
-        <v>1.6352712</v>
+        <f t="shared" si="13"/>
+        <v>22.875462487127994</v>
       </c>
       <c r="AS52" s="1">
-        <f t="shared" si="49"/>
-        <v>4.4538659999999997</v>
+        <f t="shared" si="13"/>
+        <v>37.752312776835275</v>
       </c>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.25">
@@ -5146,146 +5281,146 @@
         <v>7</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="14"/>
-        <v>7.2259740000000003E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.8086502056190366</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="14"/>
-        <v>0.27258840000000001</v>
+        <f t="shared" si="8"/>
+        <v>9.3396085571077343</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="14"/>
-        <v>0.36125820000000003</v>
+        <f t="shared" si="8"/>
+        <v>10.751866070594444</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1">
-        <f t="shared" ref="G53:L53" si="50">G22*180</f>
-        <v>1.0041983999999999E-5</v>
+        <f t="shared" ref="G53:AS53" si="14">SQRT(G22)*240</f>
+        <v>5.6687166801666848E-2</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="50"/>
-        <v>0.64440900000000001</v>
+        <f t="shared" si="14"/>
+        <v>14.360044568175963</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="50"/>
-        <v>1.6798895999999999</v>
+        <f t="shared" si="14"/>
+        <v>23.185440949009358</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1">
-        <f t="shared" si="50"/>
-        <v>7.2259740000000003E-2</v>
+        <f t="shared" si="14"/>
+        <v>4.8086502056190366</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" si="50"/>
-        <v>0.27258840000000001</v>
+        <f t="shared" si="14"/>
+        <v>9.3396085571077343</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" ref="M53" si="51">M22*180</f>
-        <v>0.36125820000000003</v>
+        <f t="shared" si="14"/>
+        <v>10.751866070594444</v>
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1">
-        <f t="shared" ref="O53:S53" si="52">O22*180</f>
-        <v>2.0424779999999998E-7</v>
+        <f t="shared" si="14"/>
+        <v>8.0845096326246021E-3</v>
       </c>
       <c r="P53" s="1">
-        <f t="shared" si="52"/>
-        <v>0.44958419999999999</v>
+        <f t="shared" si="14"/>
+        <v>11.994454718743992</v>
       </c>
       <c r="Q53" s="1">
-        <f t="shared" si="52"/>
-        <v>0.75314160000000008</v>
+        <f t="shared" si="14"/>
+        <v>15.524345783317248</v>
       </c>
       <c r="R53" s="1"/>
       <c r="S53" s="1">
-        <f t="shared" si="52"/>
-        <v>3.1023360000000002E-4</v>
+        <f t="shared" si="14"/>
+        <v>0.31507896153186743</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" ref="T53" si="53">T22*180</f>
-        <v>1.2575429999999999</v>
+        <f t="shared" si="14"/>
+        <v>20.060253238680712</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" ref="U53:W53" si="54">U22*180</f>
-        <v>0.9731322</v>
+        <f t="shared" si="14"/>
+        <v>17.646594685661025</v>
       </c>
       <c r="V53" s="1"/>
       <c r="W53" s="1">
-        <f t="shared" si="54"/>
-        <v>1.323234</v>
+        <f t="shared" si="14"/>
+        <v>20.577533379878162</v>
       </c>
       <c r="X53" s="1">
-        <f t="shared" ref="X53:Y53" si="55">X22*180</f>
-        <v>2.2754159999999999</v>
+        <f t="shared" si="14"/>
+        <v>26.983941891428689</v>
       </c>
       <c r="Y53" s="1">
-        <f t="shared" si="55"/>
-        <v>1.4843915999999999</v>
+        <f t="shared" si="14"/>
+        <v>21.79461658300049</v>
       </c>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1">
-        <f t="shared" ref="AA53:AS53" si="56">AA22*180</f>
-        <v>1.2181625999999999</v>
+        <f t="shared" si="14"/>
+        <v>19.743658019728766</v>
       </c>
       <c r="AB53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.2674844000000001</v>
+        <f t="shared" si="14"/>
+        <v>20.139389464430145</v>
       </c>
       <c r="AC53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.1702232000000001</v>
+        <f t="shared" si="14"/>
+        <v>19.351264144752921</v>
       </c>
       <c r="AD53" s="1"/>
       <c r="AE53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.2092111999999999</v>
+        <f t="shared" si="14"/>
+        <v>19.670983300282678</v>
       </c>
       <c r="AF53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.75206340000000005</v>
+        <f t="shared" si="14"/>
+        <v>15.513229451020184</v>
       </c>
       <c r="AG53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.0633158</v>
+        <f t="shared" si="14"/>
+        <v>18.446166430995898</v>
       </c>
       <c r="AH53" s="1"/>
       <c r="AI53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.10380780000000001</v>
+        <f t="shared" si="14"/>
+        <v>5.7635489067067001</v>
       </c>
       <c r="AJ53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.38754</v>
+        <f t="shared" si="14"/>
+        <v>11.136103447795373</v>
       </c>
       <c r="AK53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.3856598</v>
+        <f t="shared" si="14"/>
+        <v>21.057329745245479</v>
       </c>
       <c r="AL53" s="1"/>
       <c r="AM53" s="1">
-        <f t="shared" si="56"/>
-        <v>3.341214E-2</v>
+        <f t="shared" si="14"/>
+        <v>3.2698447669575996</v>
       </c>
       <c r="AN53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.41560739999999996</v>
+        <f t="shared" si="14"/>
+        <v>11.53231841391834</v>
       </c>
       <c r="AO53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.88144200000000006</v>
+        <f t="shared" si="14"/>
+        <v>16.794684873494948</v>
       </c>
       <c r="AP53" s="1"/>
       <c r="AQ53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.25353540000000002</v>
+        <f t="shared" si="14"/>
+        <v>9.0072930450829691</v>
       </c>
       <c r="AR53" s="1">
-        <f t="shared" si="56"/>
-        <v>1.14255</v>
+        <f t="shared" si="14"/>
+        <v>19.121087835162516</v>
       </c>
       <c r="AS53" s="1">
-        <f t="shared" si="56"/>
-        <v>0.82533600000000007</v>
+        <f t="shared" si="14"/>
+        <v>16.251385171732284</v>
       </c>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.25">
@@ -5293,146 +5428,146 @@
         <v>8</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="14"/>
-        <v>0.48022559999999997</v>
+        <f t="shared" si="8"/>
+        <v>12.39645884920367</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="14"/>
-        <v>3.1847759999999998</v>
+        <f t="shared" si="8"/>
+        <v>31.923789248771833</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="14"/>
-        <v>3.8288340000000001</v>
+        <f t="shared" si="8"/>
+        <v>35.003240992799512</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1">
-        <f t="shared" ref="G54:L54" si="57">G23*180</f>
-        <v>2.1562020000000001E-2</v>
+        <f t="shared" ref="G54:AS54" si="15">SQRT(G23)*240</f>
+        <v>2.6267558698897009</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="57"/>
-        <v>1.1618352000000001</v>
+        <f t="shared" si="15"/>
+        <v>19.281785809410913</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="57"/>
-        <v>0.4560786</v>
+        <f t="shared" si="15"/>
+        <v>12.080776134007285</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1">
-        <f t="shared" si="57"/>
-        <v>7.0477019999999998E-9</v>
+        <f t="shared" si="15"/>
+        <v>1.5017538546646051E-3</v>
       </c>
       <c r="L54" s="1">
-        <f t="shared" si="57"/>
-        <v>0.40019220000000005</v>
+        <f t="shared" si="15"/>
+        <v>11.316426291016082</v>
       </c>
       <c r="M54" s="1">
-        <f t="shared" ref="M54" si="58">M23*180</f>
-        <v>0.8473986</v>
+        <f t="shared" si="15"/>
+        <v>16.467165876373507</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1">
-        <f t="shared" ref="O54:S54" si="59">O23*180</f>
-        <v>0.33769979999999999</v>
+        <f t="shared" si="15"/>
+        <v>10.395380512516125</v>
       </c>
       <c r="P54" s="1">
-        <f t="shared" si="59"/>
-        <v>0.83142359999999993</v>
+        <f t="shared" si="15"/>
+        <v>16.311209397221283</v>
       </c>
       <c r="Q54" s="1">
-        <f t="shared" si="59"/>
-        <v>1.8124379999999998</v>
+        <f t="shared" si="15"/>
+        <v>24.08277724848195</v>
       </c>
       <c r="R54" s="1"/>
       <c r="S54" s="1">
-        <f t="shared" si="59"/>
-        <v>0.56498039999999994</v>
+        <f t="shared" si="15"/>
+        <v>13.445955823220602</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" ref="T54" si="60">T23*180</f>
-        <v>1.0304514</v>
+        <f t="shared" si="15"/>
+        <v>18.158866925003881</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" ref="U54:W54" si="61">U23*180</f>
-        <v>3.973176</v>
+        <f t="shared" si="15"/>
+        <v>35.656925274061422</v>
       </c>
       <c r="V54" s="1"/>
       <c r="W54" s="1">
-        <f t="shared" si="61"/>
-        <v>0.48896459999999997</v>
+        <f t="shared" si="15"/>
+        <v>12.508743821823195</v>
       </c>
       <c r="X54" s="1">
-        <f t="shared" ref="X54:Y54" si="62">X23*180</f>
-        <v>1.2318245999999999</v>
+        <f t="shared" si="15"/>
+        <v>19.854064369795921</v>
       </c>
       <c r="Y54" s="1">
-        <f t="shared" si="62"/>
-        <v>1.2318875999999999</v>
+        <f t="shared" si="15"/>
+        <v>19.85457206791423</v>
       </c>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1">
-        <f t="shared" ref="AA54:AS54" si="63">AA23*180</f>
-        <v>1.836468E-13</v>
+        <f t="shared" si="15"/>
+        <v>7.6659621705301924E-6</v>
       </c>
       <c r="AB54" s="1">
-        <f t="shared" si="63"/>
-        <v>0.69902639999999994</v>
+        <f t="shared" si="15"/>
+        <v>14.956217703684311</v>
       </c>
       <c r="AC54" s="1">
-        <f t="shared" si="63"/>
-        <v>1.5612372000000001</v>
+        <f t="shared" si="15"/>
+        <v>22.351642087327722</v>
       </c>
       <c r="AD54" s="1"/>
       <c r="AE54" s="1">
-        <f t="shared" si="63"/>
-        <v>1.036467</v>
+        <f t="shared" si="15"/>
+        <v>18.211793980824623</v>
       </c>
       <c r="AF54" s="1">
-        <f t="shared" si="63"/>
-        <v>2.0648879999999998</v>
+        <f t="shared" si="15"/>
+        <v>25.705333298753395</v>
       </c>
       <c r="AG54" s="1">
-        <f t="shared" si="63"/>
-        <v>2.1781079999999999</v>
+        <f t="shared" si="15"/>
+        <v>26.400654537340547</v>
       </c>
       <c r="AH54" s="1"/>
       <c r="AI54" s="1">
-        <f t="shared" si="63"/>
-        <v>3.0545820000000003E-8</v>
+        <f t="shared" si="15"/>
+        <v>3.1264456496155504E-3</v>
       </c>
       <c r="AJ54" s="1">
-        <f t="shared" si="63"/>
-        <v>3.4104599999999996</v>
+        <f t="shared" si="15"/>
+        <v>33.035544493772157</v>
       </c>
       <c r="AK54" s="1">
-        <f t="shared" si="63"/>
-        <v>1.6583400000000001</v>
+        <f t="shared" si="15"/>
+        <v>23.036249694774536</v>
       </c>
       <c r="AL54" s="1"/>
       <c r="AM54" s="1">
-        <f t="shared" si="63"/>
-        <v>1.8918539999999999</v>
+        <f t="shared" si="15"/>
+        <v>24.604741006562129</v>
       </c>
       <c r="AN54" s="1">
-        <f t="shared" si="63"/>
-        <v>2.8096739999999998</v>
+        <f t="shared" si="15"/>
+        <v>29.984924212010274</v>
       </c>
       <c r="AO54" s="1">
-        <f t="shared" si="63"/>
-        <v>4.020696</v>
+        <f t="shared" si="15"/>
+        <v>35.869523554125998</v>
       </c>
       <c r="AP54" s="1"/>
       <c r="AQ54" s="1">
-        <f t="shared" si="63"/>
-        <v>2.1556260000000003</v>
+        <f t="shared" si="15"/>
+        <v>26.264049954262575</v>
       </c>
       <c r="AR54" s="1">
-        <f t="shared" si="63"/>
-        <v>2.7536580000000002</v>
+        <f t="shared" si="15"/>
+        <v>29.684517176467601</v>
       </c>
       <c r="AS54" s="1">
-        <f t="shared" si="63"/>
-        <v>3.5989559999999998</v>
+        <f t="shared" si="15"/>
+        <v>33.936203676899396</v>
       </c>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.25">
@@ -5440,146 +5575,146 @@
         <v>9</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="14"/>
-        <v>0.6789636</v>
+        <f t="shared" si="8"/>
+        <v>14.740025508797466</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="14"/>
-        <v>0.62577720000000003</v>
+        <f t="shared" si="8"/>
+        <v>14.150925906102399</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="14"/>
-        <v>1.2279978</v>
+        <f t="shared" si="8"/>
+        <v>19.823200952419366</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1">
-        <f t="shared" ref="G55:L55" si="64">G24*180</f>
-        <v>0.87998940000000003</v>
+        <f t="shared" ref="G55:AS55" si="16">SQRT(G24)*240</f>
+        <v>16.780840503383612</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="64"/>
-        <v>1.810908</v>
+        <f t="shared" si="16"/>
+        <v>24.072610161758529</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="64"/>
-        <v>2.2437359999999997</v>
+        <f t="shared" si="16"/>
+        <v>26.795438417760586</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1">
-        <f t="shared" si="64"/>
-        <v>0.48022559999999997</v>
+        <f t="shared" si="16"/>
+        <v>12.39645884920367</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" si="64"/>
-        <v>3.1848120000000004</v>
+        <f t="shared" si="16"/>
+        <v>31.923969677970813</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" ref="M55" si="65">M24*180</f>
-        <v>3.8288340000000001</v>
+        <f t="shared" si="16"/>
+        <v>35.003240992799512</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1">
-        <f t="shared" ref="O55:S55" si="66">O24*180</f>
-        <v>7.3786499999999996E-5</v>
+        <f t="shared" si="16"/>
+        <v>0.15366092541697124</v>
       </c>
       <c r="P55" s="1">
-        <f t="shared" si="66"/>
-        <v>1.4913198000000001</v>
+        <f t="shared" si="16"/>
+        <v>21.845419107904522</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="66"/>
-        <v>0.87507000000000001</v>
+        <f t="shared" si="16"/>
+        <v>16.733869845316715</v>
       </c>
       <c r="R55" s="1"/>
       <c r="S55" s="1">
-        <f t="shared" si="66"/>
-        <v>0.86630399999999996</v>
+        <f t="shared" si="16"/>
+        <v>16.649843242505316</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" ref="T55" si="67">T24*180</f>
-        <v>2.4551460000000001</v>
+        <f t="shared" si="16"/>
+        <v>28.029390289480077</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" ref="U55:W55" si="68">U24*180</f>
-        <v>3.4102800000000002</v>
+        <f t="shared" si="16"/>
+        <v>33.034672694004399</v>
       </c>
       <c r="V55" s="1"/>
       <c r="W55" s="1">
-        <f t="shared" si="68"/>
-        <v>3.0419099999999998E-2</v>
+        <f t="shared" si="16"/>
+        <v>3.1199538458124665</v>
       </c>
       <c r="X55" s="1">
-        <f t="shared" ref="X55:Y55" si="69">X24*180</f>
-        <v>0.84456719999999996</v>
+        <f t="shared" si="16"/>
+        <v>16.439632112672108</v>
       </c>
       <c r="Y55" s="1">
-        <f t="shared" si="69"/>
-        <v>0.75603059999999989</v>
+        <f t="shared" si="16"/>
+        <v>15.554092451827589</v>
       </c>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1">
-        <f t="shared" ref="AA55:AS55" si="70">AA24*180</f>
-        <v>0.29804940000000002</v>
+        <f t="shared" si="16"/>
+        <v>9.7660538601832414</v>
       </c>
       <c r="AB55" s="1">
-        <f t="shared" si="70"/>
-        <v>4.1425380000000001</v>
+        <f t="shared" si="16"/>
+        <v>36.40895713969298</v>
       </c>
       <c r="AC55" s="1">
-        <f t="shared" si="70"/>
-        <v>4.6755180000000003</v>
+        <f t="shared" si="16"/>
+        <v>38.680301963661037</v>
       </c>
       <c r="AD55" s="1"/>
       <c r="AE55" s="1">
-        <f t="shared" si="70"/>
-        <v>0.20293919999999999</v>
+        <f t="shared" si="16"/>
+        <v>8.058569600121352</v>
       </c>
       <c r="AF55" s="1">
-        <f t="shared" si="70"/>
-        <v>2.6188380000000002</v>
+        <f t="shared" si="16"/>
+        <v>28.948716033703466</v>
       </c>
       <c r="AG55" s="1">
-        <f t="shared" si="70"/>
-        <v>3.2329619999999997</v>
+        <f t="shared" si="16"/>
+        <v>32.164387760378716</v>
       </c>
       <c r="AH55" s="1"/>
       <c r="AI55" s="1">
-        <f t="shared" si="70"/>
-        <v>0.12572514000000001</v>
+        <f t="shared" si="16"/>
+        <v>6.342873544380339</v>
       </c>
       <c r="AJ55" s="1">
-        <f t="shared" si="70"/>
-        <v>3.0774780000000002</v>
+        <f t="shared" si="16"/>
+        <v>31.381411058140774</v>
       </c>
       <c r="AK55" s="1">
-        <f t="shared" si="70"/>
-        <v>3.1570019999999999</v>
+        <f t="shared" si="16"/>
+        <v>31.784282908380991</v>
       </c>
       <c r="AL55" s="1"/>
       <c r="AM55" s="1">
-        <f t="shared" si="70"/>
-        <v>0.2144916</v>
+        <f t="shared" si="16"/>
+        <v>8.2847638469663085</v>
       </c>
       <c r="AN55" s="1">
-        <f t="shared" si="70"/>
-        <v>3.299544</v>
+        <f t="shared" si="16"/>
+        <v>32.493908352181947</v>
       </c>
       <c r="AO55" s="1">
-        <f t="shared" si="70"/>
-        <v>4.8876299999999997</v>
+        <f t="shared" si="16"/>
+        <v>39.547965813679973</v>
       </c>
       <c r="AP55" s="1"/>
       <c r="AQ55" s="1">
-        <f t="shared" si="70"/>
-        <v>0.642015</v>
+        <f t="shared" si="16"/>
+        <v>14.333345736428742</v>
       </c>
       <c r="AR55" s="1">
-        <f t="shared" si="70"/>
-        <v>6.2554680000000005</v>
+        <f t="shared" si="16"/>
+        <v>44.740918184588033</v>
       </c>
       <c r="AS55" s="1">
-        <f t="shared" si="70"/>
-        <v>2.6438760000000001</v>
+        <f t="shared" si="16"/>
+        <v>29.086772251317264</v>
       </c>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.25">
@@ -5587,146 +5722,146 @@
         <v>10</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="14"/>
-        <v>0.63368100000000005</v>
+        <f t="shared" si="8"/>
+        <v>14.240011235950623</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="14"/>
-        <v>1.0798542</v>
+        <f t="shared" si="8"/>
+        <v>18.589065172837497</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="14"/>
-        <v>0.84384000000000003</v>
+        <f t="shared" si="8"/>
+        <v>16.432553057878742</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1">
-        <f t="shared" ref="G56:L56" si="71">G25*180</f>
-        <v>1.8631440000000001</v>
+        <f t="shared" ref="G56:AS56" si="17">SQRT(G25)*240</f>
+        <v>24.417331549536694</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="71"/>
-        <v>1.8403019999999999</v>
+        <f t="shared" si="17"/>
+        <v>24.267192668291894</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="71"/>
-        <v>2.8733580000000001</v>
+        <f t="shared" si="17"/>
+        <v>30.322838917225411</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1">
-        <f t="shared" si="71"/>
-        <v>0.6789636</v>
+        <f t="shared" si="17"/>
+        <v>14.740025508797466</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" si="71"/>
-        <v>0.62577720000000003</v>
+        <f t="shared" si="17"/>
+        <v>14.150925906102399</v>
       </c>
       <c r="M56" s="1">
-        <f t="shared" ref="M56" si="72">M25*180</f>
-        <v>1.2279978</v>
+        <f t="shared" si="17"/>
+        <v>19.823200952419366</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1">
-        <f t="shared" ref="O56:S56" si="73">O25*180</f>
-        <v>1.0974168000000001E-2</v>
+        <f t="shared" si="17"/>
+        <v>1.8739620487085644</v>
       </c>
       <c r="P56" s="1">
-        <f t="shared" si="73"/>
-        <v>1.1129777999999999</v>
+        <f t="shared" si="17"/>
+        <v>18.872013565065068</v>
       </c>
       <c r="Q56" s="1">
-        <f t="shared" si="73"/>
-        <v>2.7762480000000003</v>
+        <f t="shared" si="17"/>
+        <v>29.806028920337575</v>
       </c>
       <c r="R56" s="1"/>
       <c r="S56" s="1">
-        <f t="shared" si="73"/>
-        <v>3.3669359999999997E-5</v>
+        <f t="shared" si="17"/>
+        <v>0.10379882080255055</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" ref="T56" si="74">T25*180</f>
-        <v>4.8702059999999996</v>
+        <f t="shared" si="17"/>
+        <v>39.477410249407193</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" ref="U56:W56" si="75">U25*180</f>
-        <v>1.5377921999999999</v>
+        <f t="shared" si="17"/>
+        <v>22.183180655622852</v>
       </c>
       <c r="V56" s="1"/>
       <c r="W56" s="1">
-        <f t="shared" si="75"/>
-        <v>1.039158</v>
+        <f t="shared" si="17"/>
+        <v>18.235420477740565</v>
       </c>
       <c r="X56" s="1">
-        <f t="shared" ref="X56:Y56" si="76">X25*180</f>
-        <v>1.5802254</v>
+        <f t="shared" si="17"/>
+        <v>22.487154733313861</v>
       </c>
       <c r="Y56" s="1">
-        <f t="shared" si="76"/>
-        <v>3.1192380000000002</v>
+        <f t="shared" si="17"/>
+        <v>31.593609480399675</v>
       </c>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1">
-        <f t="shared" ref="AA56:AS56" si="77">AA25*180</f>
-        <v>7.6059000000000012E-7</v>
+        <f t="shared" si="17"/>
+        <v>1.5600923049614726E-2</v>
       </c>
       <c r="AB56" s="1">
-        <f t="shared" si="77"/>
-        <v>0.58342859999999996</v>
+        <f t="shared" si="17"/>
+        <v>13.663716624696224</v>
       </c>
       <c r="AC56" s="1">
-        <f t="shared" si="77"/>
-        <v>3.7666979999999999</v>
+        <f t="shared" si="17"/>
+        <v>34.718055245073849</v>
       </c>
       <c r="AD56" s="1"/>
       <c r="AE56" s="1">
-        <f t="shared" si="77"/>
-        <v>8.6437079999999999E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.6631255394587625</v>
       </c>
       <c r="AF56" s="1">
-        <f t="shared" si="77"/>
-        <v>0.79910460000000005</v>
+        <f t="shared" si="17"/>
+        <v>15.991043493155788</v>
       </c>
       <c r="AG56" s="1">
-        <f t="shared" si="77"/>
-        <v>2.3452920000000002</v>
+        <f t="shared" si="17"/>
+        <v>27.395135334580846</v>
       </c>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1">
-        <f t="shared" si="77"/>
-        <v>0.21606300000000001</v>
+        <f t="shared" si="17"/>
+        <v>8.3150562235020384</v>
       </c>
       <c r="AJ56" s="1">
-        <f t="shared" si="77"/>
-        <v>0.68422859999999996</v>
+        <f t="shared" si="17"/>
+        <v>14.79706565505472</v>
       </c>
       <c r="AK56" s="1">
-        <f t="shared" si="77"/>
-        <v>4.1982660000000003</v>
+        <f t="shared" si="17"/>
+        <v>36.653036981947352</v>
       </c>
       <c r="AL56" s="1"/>
       <c r="AM56" s="1">
-        <f t="shared" si="77"/>
-        <v>5.1272999999999997E-18</v>
+        <f t="shared" si="17"/>
+        <v>4.0505999555621388E-8</v>
       </c>
       <c r="AN56" s="1">
-        <f t="shared" si="77"/>
-        <v>1.0176984</v>
+        <f t="shared" si="17"/>
+        <v>18.0461488412348</v>
       </c>
       <c r="AO56" s="1">
-        <f t="shared" si="77"/>
-        <v>3.6205020000000001</v>
+        <f t="shared" si="17"/>
+        <v>34.037635640567046</v>
       </c>
       <c r="AP56" s="1"/>
       <c r="AQ56" s="1">
-        <f t="shared" si="77"/>
-        <v>0.23261039999999999</v>
+        <f t="shared" si="17"/>
+        <v>8.6275910890584058</v>
       </c>
       <c r="AR56" s="1">
-        <f t="shared" si="77"/>
-        <v>1.404954</v>
+        <f t="shared" si="17"/>
+        <v>21.203426138244733</v>
       </c>
       <c r="AS56" s="1">
-        <f t="shared" si="77"/>
-        <v>2.276046</v>
+        <f t="shared" si="17"/>
+        <v>26.987677187931531</v>
       </c>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.25">
@@ -5810,145 +5945,145 @@
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(C47:C56)</f>
-        <v>0.24754239180000001</v>
+        <v>7.7914107114669449</v>
       </c>
       <c r="D73" s="5">
-        <f t="shared" ref="D73:E73" si="78">AVERAGE(D47:D56)</f>
-        <v>1.2322834199999999</v>
+        <f t="shared" ref="D73:E73" si="18">AVERAGE(D47:D56)</f>
+        <v>19.056484162607024</v>
       </c>
       <c r="E73" s="5">
-        <f t="shared" si="78"/>
-        <v>1.30328226</v>
+        <f t="shared" si="18"/>
+        <v>19.239361600118862</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5">
-        <f t="shared" ref="G73:I73" si="79">AVERAGE(G47:G56)</f>
-        <v>0.46965892119839997</v>
+        <f t="shared" ref="G73:I73" si="19">AVERAGE(G47:G56)</f>
+        <v>9.8833765116237835</v>
       </c>
       <c r="H73" s="5">
-        <f t="shared" si="79"/>
-        <v>1.18919826</v>
+        <f t="shared" si="19"/>
+        <v>18.555301703416632</v>
       </c>
       <c r="I73" s="5">
-        <f t="shared" si="79"/>
-        <v>1.5640482599999999</v>
+        <f t="shared" si="19"/>
+        <v>21.740096738030765</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5">
-        <f t="shared" ref="K73:S73" si="80">AVERAGE(K47:K56)</f>
-        <v>0.18417429250477019</v>
+        <f t="shared" ref="K73:S73" si="20">AVERAGE(K47:K56)</f>
+        <v>6.3675597632573488</v>
       </c>
       <c r="L73" s="5">
-        <f t="shared" si="80"/>
-        <v>1.1643208199999999</v>
+        <f t="shared" si="20"/>
+        <v>18.329238317344778</v>
       </c>
       <c r="M73" s="5">
-        <f t="shared" si="80"/>
-        <v>1.30363308</v>
+        <f t="shared" si="20"/>
+        <v>19.24276581904774</v>
       </c>
       <c r="N73" s="5"/>
       <c r="O73" s="5">
-        <f t="shared" si="80"/>
-        <v>0.20378195676521926</v>
+        <f t="shared" si="20"/>
+        <v>4.6187312049853064</v>
       </c>
       <c r="P73" s="5">
-        <f t="shared" si="80"/>
-        <v>1.2302083799999999</v>
+        <f t="shared" si="20"/>
+        <v>18.746940836865697</v>
       </c>
       <c r="Q73" s="5">
-        <f t="shared" si="80"/>
-        <v>1.4668761600000002</v>
+        <f t="shared" si="20"/>
+        <v>21.086478511313221</v>
       </c>
       <c r="R73" s="5"/>
       <c r="S73" s="5">
-        <f t="shared" si="80"/>
-        <v>0.59497052973839992</v>
+        <f t="shared" si="20"/>
+        <v>10.513793516962274</v>
       </c>
       <c r="T73" s="5">
-        <f t="shared" ref="T73:U73" si="81">AVERAGE(T47:T56)</f>
-        <v>2.3177989800000001</v>
+        <f t="shared" ref="T73:U73" si="21">AVERAGE(T47:T56)</f>
+        <v>26.140237961089223</v>
       </c>
       <c r="U73" s="5">
-        <f t="shared" si="81"/>
-        <v>2.5174241999999998</v>
+        <f t="shared" si="21"/>
+        <v>27.535276343664911</v>
       </c>
       <c r="V73" s="5"/>
       <c r="W73" s="5">
-        <f t="shared" ref="W73:Y73" si="82">AVERAGE(W47:W56)</f>
-        <v>0.55760841751244394</v>
+        <f t="shared" ref="W73:Y73" si="22">AVERAGE(W47:W56)</f>
+        <v>10.88014638498794</v>
       </c>
       <c r="X73" s="5">
-        <f t="shared" si="82"/>
-        <v>1.4235393599999999</v>
+        <f t="shared" si="22"/>
+        <v>20.933793351349742</v>
       </c>
       <c r="Y73" s="5">
-        <f t="shared" si="82"/>
-        <v>2.2340986199999997</v>
+        <f t="shared" si="22"/>
+        <v>25.4981907079157</v>
       </c>
       <c r="Z73" s="5"/>
       <c r="AA73" s="5">
-        <f t="shared" ref="AA73:AS73" si="83">AVERAGE(AA47:AA56)</f>
-        <v>0.28466215965904068</v>
+        <f t="shared" ref="AA73:AS73" si="23">AVERAGE(AA47:AA56)</f>
+        <v>5.9757212857751103</v>
       </c>
       <c r="AB73" s="5">
-        <f t="shared" si="83"/>
-        <v>1.56164364</v>
+        <f t="shared" si="23"/>
+        <v>21.550319558775762</v>
       </c>
       <c r="AC73" s="5">
-        <f t="shared" si="83"/>
-        <v>2.3575332600000003</v>
+        <f t="shared" si="23"/>
+        <v>26.785021859966616</v>
       </c>
       <c r="AD73" s="5"/>
       <c r="AE73" s="5">
-        <f t="shared" si="83"/>
-        <v>0.41583975480000007</v>
+        <f t="shared" si="23"/>
+        <v>9.2442465212309557</v>
       </c>
       <c r="AF73" s="5">
-        <f t="shared" si="83"/>
-        <v>1.5992967600000001</v>
+        <f t="shared" si="23"/>
+        <v>22.25940464059104</v>
       </c>
       <c r="AG73" s="5">
-        <f t="shared" si="83"/>
-        <v>1.8482945400000002</v>
+        <f t="shared" si="23"/>
+        <v>23.9577637103901</v>
       </c>
       <c r="AH73" s="5"/>
       <c r="AI73" s="5">
-        <f t="shared" si="83"/>
-        <v>0.17094831965458201</v>
+        <f t="shared" si="23"/>
+        <v>5.3380232370172909</v>
       </c>
       <c r="AJ73" s="5">
-        <f t="shared" si="83"/>
-        <v>1.6890883200000002</v>
+        <f t="shared" si="23"/>
+        <v>22.179561461675494</v>
       </c>
       <c r="AK73" s="5">
-        <f t="shared" si="83"/>
-        <v>2.19550482</v>
+        <f t="shared" si="23"/>
+        <v>25.712709585538516</v>
       </c>
       <c r="AL73" s="5"/>
       <c r="AM73" s="5">
-        <f t="shared" si="83"/>
-        <v>0.4825851298199999</v>
+        <f t="shared" si="23"/>
+        <v>8.7199966505058768</v>
       </c>
       <c r="AN73" s="5">
-        <f t="shared" si="83"/>
-        <v>1.7704078200000002</v>
+        <f t="shared" si="23"/>
+        <v>23.056498796356102</v>
       </c>
       <c r="AO73" s="5">
-        <f t="shared" si="83"/>
-        <v>2.652228</v>
+        <f t="shared" si="23"/>
+        <v>28.135422506334869</v>
       </c>
       <c r="AP73" s="5"/>
       <c r="AQ73" s="5">
-        <f t="shared" si="83"/>
-        <v>0.43908192336600005</v>
+        <f t="shared" si="23"/>
+        <v>9.244558994369438</v>
       </c>
       <c r="AR73" s="5">
-        <f t="shared" si="83"/>
-        <v>2.5330174200000002</v>
+        <f t="shared" si="23"/>
+        <v>27.643338631241573</v>
       </c>
       <c r="AS73" s="5">
-        <f t="shared" si="83"/>
-        <v>2.3886489599999998</v>
+        <f t="shared" si="23"/>
+        <v>27.040128453324151</v>
       </c>
     </row>
     <row r="74" spans="1:45" x14ac:dyDescent="0.25">
@@ -5957,135 +6092,135 @@
       </c>
       <c r="C74">
         <f>_xlfn.STDEV.S(C47:C56)</f>
-        <v>0.25101165429320771</v>
+        <v>4.5347405292962888</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:E74" si="84">_xlfn.STDEV.S(D47:D56)</f>
-        <v>0.78445209414837025</v>
+        <f t="shared" ref="D74:E74" si="24">_xlfn.STDEV.S(D47:D56)</f>
+        <v>5.8860575147553966</v>
       </c>
       <c r="E74">
-        <f t="shared" si="84"/>
-        <v>1.0418522284963234</v>
+        <f t="shared" si="24"/>
+        <v>7.218593924325007</v>
       </c>
       <c r="G74">
-        <f t="shared" ref="G74:I74" si="85">_xlfn.STDEV.S(G47:G56)</f>
-        <v>0.57670023830322381</v>
+        <f t="shared" ref="G74:I74" si="25">_xlfn.STDEV.S(G47:G56)</f>
+        <v>7.6456032036554076</v>
       </c>
       <c r="H74">
-        <f t="shared" si="85"/>
-        <v>0.73060226892751701</v>
+        <f t="shared" si="25"/>
+        <v>6.3459717665078967</v>
       </c>
       <c r="I74">
-        <f t="shared" si="85"/>
-        <v>0.73538780367365142</v>
+        <f t="shared" si="25"/>
+        <v>5.5641348554893346</v>
       </c>
       <c r="K74">
-        <f t="shared" ref="K74:S74" si="86">_xlfn.STDEV.S(K47:K56)</f>
-        <v>0.22087721645556738</v>
+        <f t="shared" ref="K74:S74" si="26">_xlfn.STDEV.S(K47:K56)</f>
+        <v>4.5203190967590947</v>
       </c>
       <c r="L74">
-        <f t="shared" si="86"/>
-        <v>0.82740413034376614</v>
+        <f t="shared" si="26"/>
+        <v>6.3789310412377596</v>
       </c>
       <c r="M74">
-        <f t="shared" si="86"/>
-        <v>1.0416816642410021</v>
+        <f t="shared" si="26"/>
+        <v>7.2171515798045709</v>
       </c>
       <c r="O74">
-        <f t="shared" si="86"/>
-        <v>0.45411941619999818</v>
+        <f t="shared" si="26"/>
+        <v>6.9823227766000562</v>
       </c>
       <c r="P74">
-        <f t="shared" si="86"/>
-        <v>0.84534644750857302</v>
+        <f t="shared" si="26"/>
+        <v>6.8490786776241563</v>
       </c>
       <c r="Q74">
-        <f t="shared" si="86"/>
-        <v>0.72250033002512593</v>
+        <f t="shared" si="26"/>
+        <v>5.2451877619104579</v>
       </c>
       <c r="S74">
-        <f t="shared" si="86"/>
-        <v>0.61596199655174544</v>
+        <f t="shared" si="26"/>
+        <v>9.4192896287335142</v>
       </c>
       <c r="T74">
-        <f t="shared" ref="T74:U74" si="87">_xlfn.STDEV.S(T47:T56)</f>
-        <v>1.4144738554931318</v>
+        <f t="shared" ref="T74:U74" si="27">_xlfn.STDEV.S(T47:T56)</f>
+        <v>8.0542351135308419</v>
       </c>
       <c r="U74">
-        <f t="shared" si="87"/>
-        <v>1.2523707420669654</v>
+        <f t="shared" si="27"/>
+        <v>7.2559784299268655</v>
       </c>
       <c r="W74">
-        <f t="shared" ref="W74:Y74" si="88">_xlfn.STDEV.S(W47:W56)</f>
-        <v>0.54503640204399961</v>
+        <f t="shared" ref="W74:Y74" si="28">_xlfn.STDEV.S(W47:W56)</f>
+        <v>8.1688506090185147</v>
       </c>
       <c r="X74">
-        <f t="shared" si="88"/>
-        <v>0.59230002885100019</v>
+        <f t="shared" si="28"/>
+        <v>4.3854419672093963</v>
       </c>
       <c r="Y74">
-        <f t="shared" si="88"/>
-        <v>1.6043563852196951</v>
+        <f t="shared" si="28"/>
+        <v>8.4822578901009233</v>
       </c>
       <c r="AA74">
-        <f t="shared" ref="AA74:AS74" si="89">_xlfn.STDEV.S(AA47:AA56)</f>
-        <v>0.49622545964097092</v>
+        <f t="shared" ref="AA74:AS74" si="29">_xlfn.STDEV.S(AA47:AA56)</f>
+        <v>7.8445059475921166</v>
       </c>
       <c r="AB74">
-        <f t="shared" si="89"/>
-        <v>0.99565132889835284</v>
+        <f t="shared" si="29"/>
+        <v>6.2636244135525843</v>
       </c>
       <c r="AC74">
-        <f t="shared" si="89"/>
-        <v>1.1510664731392859</v>
+        <f t="shared" si="29"/>
+        <v>6.4094762449491256</v>
       </c>
       <c r="AE74">
-        <f t="shared" si="89"/>
-        <v>0.49661371798923826</v>
+        <f t="shared" si="29"/>
+        <v>7.2734393355176135</v>
       </c>
       <c r="AF74">
-        <f t="shared" si="89"/>
-        <v>0.57717741468669403</v>
+        <f t="shared" si="29"/>
+        <v>4.254914576298038</v>
       </c>
       <c r="AG74">
-        <f t="shared" si="89"/>
-        <v>0.67427568198032706</v>
+        <f t="shared" si="29"/>
+        <v>4.4070411839231474</v>
       </c>
       <c r="AI74">
-        <f t="shared" si="89"/>
-        <v>0.29102738855365495</v>
+        <f t="shared" si="29"/>
+        <v>5.396394908797876</v>
       </c>
       <c r="AJ74">
-        <f t="shared" si="89"/>
-        <v>1.0271640805556936</v>
+        <f t="shared" si="29"/>
+        <v>7.3466028254757374</v>
       </c>
       <c r="AK74">
-        <f t="shared" si="89"/>
-        <v>1.1326796183704566</v>
+        <f t="shared" si="29"/>
+        <v>6.7838131009497609</v>
       </c>
       <c r="AM74">
-        <f t="shared" si="89"/>
-        <v>0.70528006680883459</v>
+        <f t="shared" si="29"/>
+        <v>9.3326725931337187</v>
       </c>
       <c r="AN74">
-        <f t="shared" si="89"/>
-        <v>0.88894036258876419</v>
+        <f t="shared" si="29"/>
+        <v>6.2297106811391769</v>
       </c>
       <c r="AO74">
-        <f t="shared" si="89"/>
-        <v>1.3594251876732011</v>
+        <f t="shared" si="29"/>
+        <v>7.96596652362937</v>
       </c>
       <c r="AQ74">
-        <f t="shared" si="89"/>
-        <v>0.65576149165794095</v>
+        <f t="shared" si="29"/>
+        <v>7.8205103894782209</v>
       </c>
       <c r="AR74">
-        <f t="shared" si="89"/>
-        <v>1.4465183376458668</v>
+        <f t="shared" si="29"/>
+        <v>7.181102029208124</v>
       </c>
       <c r="AS74">
-        <f t="shared" si="89"/>
-        <v>1.0467784475970925</v>
+        <f t="shared" si="29"/>
+        <v>6.0735419308971927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>